<commit_message>
create student data table
</commit_message>
<xml_diff>
--- a/sample-data.xlsx
+++ b/sample-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\karname\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4579572F-5CE8-47F4-A258-37C2D362B1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2922A771-63A5-4FC1-8CC6-6AD9FA5C89A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{80EF0736-ECAB-4203-883F-355C71502412}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{80EF0736-ECAB-4203-883F-355C71502412}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -194,6 +194,33 @@
   </si>
   <si>
     <t>اسفند 1403</t>
+  </si>
+  <si>
+    <t>تینا قربانی</t>
+  </si>
+  <si>
+    <t>راهنمایی</t>
+  </si>
+  <si>
+    <t>مهدی</t>
+  </si>
+  <si>
+    <t>الینا فیاضی</t>
+  </si>
+  <si>
+    <t>هستی رحمانی</t>
+  </si>
+  <si>
+    <t>حدیث فتح الهی</t>
+  </si>
+  <si>
+    <t>ریاضی 8</t>
+  </si>
+  <si>
+    <t>تینا</t>
+  </si>
+  <si>
+    <t>زهرا فیضی زاده</t>
   </si>
 </sst>
 </file>
@@ -550,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF5FDB3-A5B3-4338-8137-14F11F0AED91}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -609,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28987B1F-C65F-4D05-BE57-4B13ABD87443}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -810,33 +837,96 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="str">
+      <c r="A10">
         <f t="shared" si="0"/>
-        <v/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="str">
+      <c r="A11">
         <f t="shared" si="0"/>
-        <v/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="str">
+      <c r="A12">
         <f t="shared" si="0"/>
-        <v/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="1">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
+      <c r="A13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="1">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="str">
+      <c r="A14">
         <f t="shared" si="0"/>
-        <v/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1030,7 +1120,7 @@
   <dimension ref="A1:D530"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1157,9 +1247,18 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="str">
+      <c r="A9">
         <f t="shared" si="0"/>
-        <v/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4299,7 +4398,7 @@
   <dimension ref="A1:E515"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4440,53 +4539,98 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D8" t="str">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8">
         <f>IF(ISBLANK(A8),"",_xlfn.XLOOKUP(A8,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E8" t="str">
+        <v>13</v>
+      </c>
+      <c r="E8">
         <f>IF(ISBLANK(B8),"",_xlfn.XLOOKUP(B8,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D9" t="str">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9">
         <f>IF(ISBLANK(A9),"",_xlfn.XLOOKUP(A9,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E9" t="str">
+        <v>12</v>
+      </c>
+      <c r="E9">
         <f>IF(ISBLANK(B9),"",_xlfn.XLOOKUP(B9,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" t="str">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10">
         <f>IF(ISBLANK(A10),"",_xlfn.XLOOKUP(A10,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E10" t="str">
+        <v>11</v>
+      </c>
+      <c r="E10">
         <f>IF(ISBLANK(B10),"",_xlfn.XLOOKUP(B10,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D11" t="str">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11">
         <f>IF(ISBLANK(A11),"",_xlfn.XLOOKUP(A11,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E11" t="str">
+        <v>10</v>
+      </c>
+      <c r="E11">
         <f>IF(ISBLANK(B11),"",_xlfn.XLOOKUP(B11,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" t="str">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12">
         <f>IF(ISBLANK(A12),"",_xlfn.XLOOKUP(A12,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E12" t="str">
+        <v>9</v>
+      </c>
+      <c r="E12">
         <f>IF(ISBLANK(B12),"",_xlfn.XLOOKUP(B12,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -9490,7 +9634,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A89D5F-6126-46AB-8F99-3687AF635A1D}">
-  <dimension ref="A1:E667"/>
+  <dimension ref="A1:E662"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -9520,97 +9664,97 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(A2),"",_xlfn.XLOOKUP(A2,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <f>IF(ISBLANK(B2),"",_xlfn.XLOOKUP(B2,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>18.5</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(A3),"",_xlfn.XLOOKUP(A3,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <f>IF(ISBLANK(B3),"",_xlfn.XLOOKUP(B3,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(A4),"",_xlfn.XLOOKUP(A4,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <f>IF(ISBLANK(B4),"",_xlfn.XLOOKUP(B4,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>17.5</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(A5),"",_xlfn.XLOOKUP(A5,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <f>IF(ISBLANK(B5),"",_xlfn.XLOOKUP(B5,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <f>IF(ISBLANK(A6),"",_xlfn.XLOOKUP(A6,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <f>IF(ISBLANK(B6),"",_xlfn.XLOOKUP(B6,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -16170,56 +16314,6 @@
       </c>
       <c r="E662" t="str">
         <f>IF(ISBLANK(B662),"",_xlfn.XLOOKUP(B662,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="663" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D663" t="str">
-        <f>IF(ISBLANK(A663),"",_xlfn.XLOOKUP(A663,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E663" t="str">
-        <f>IF(ISBLANK(B663),"",_xlfn.XLOOKUP(B663,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="664" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D664" t="str">
-        <f>IF(ISBLANK(A664),"",_xlfn.XLOOKUP(A664,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E664" t="str">
-        <f>IF(ISBLANK(B664),"",_xlfn.XLOOKUP(B664,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="665" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D665" t="str">
-        <f>IF(ISBLANK(A665),"",_xlfn.XLOOKUP(A665,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E665" t="str">
-        <f>IF(ISBLANK(B665),"",_xlfn.XLOOKUP(B665,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="666" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D666" t="str">
-        <f>IF(ISBLANK(A666),"",_xlfn.XLOOKUP(A666,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E666" t="str">
-        <f>IF(ISBLANK(B666),"",_xlfn.XLOOKUP(B666,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="667" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D667" t="str">
-        <f>IF(ISBLANK(A667),"",_xlfn.XLOOKUP(A667,students!B:B,students!A:A,"یافت نشد"))</f>
-        <v/>
-      </c>
-      <c r="E667" t="str">
-        <f>IF(ISBLANK(B667),"",_xlfn.XLOOKUP(B667,lessons!B:B,lessons!A:A,"یافت نشد"))</f>
         <v/>
       </c>
     </row>

</xml_diff>